<commit_message>
done Q22 factorial of a large number
</commit_message>
<xml_diff>
--- a/Resources/DSA_450_LoveBabbar.xlsx
+++ b/Resources/DSA_450_LoveBabbar.xlsx
@@ -1810,10 +1810,10 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -2154,7 +2154,7 @@
       <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="16" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2169,7 +2169,7 @@
       <c r="B27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="5" t="s">

</xml_diff>

<commit_message>
done Q24 longest increasing subsequence
</commit_message>
<xml_diff>
--- a/Resources/DSA_450_LoveBabbar.xlsx
+++ b/Resources/DSA_450_LoveBabbar.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">find maximum product subarray </t>
   </si>
   <si>
-    <t xml:space="preserve">Find longest coinsecutive subsequence</t>
+    <t xml:space="preserve">Find longest consecutive subsequence</t>
   </si>
   <si>
     <t xml:space="preserve">Given an array of size n and a number k, fin all elements that appear more than " n/k " times.</t>
@@ -1810,10 +1810,10 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -2184,7 +2184,7 @@
       <c r="B28" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -2199,7 +2199,7 @@
       <c r="B29" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="5" t="s">
@@ -8818,7 +8818,7 @@
     <hyperlink ref="C26" r:id="rId22" display="Find if there is any subarray with sum equal to 0"/>
     <hyperlink ref="C27" r:id="rId23" display="Find factorial of a large number"/>
     <hyperlink ref="C28" r:id="rId24" display="find maximum product subarray "/>
-    <hyperlink ref="C29" r:id="rId25" display="Find longest coinsecutive subsequence"/>
+    <hyperlink ref="C29" r:id="rId25" display="Find longest consecutive subsequence"/>
     <hyperlink ref="C30" r:id="rId26" display="Given an array of size n and a number k, fin all elements that appear more than &quot; n/k &quot; times."/>
     <hyperlink ref="C31" r:id="rId27" display="Maximum profit by buying and selling a share atmost twice"/>
     <hyperlink ref="C32" r:id="rId28" display="Find whether an array is a subset of another array"/>

</xml_diff>

<commit_message>
done Q26 trade stocks two times a day
</commit_message>
<xml_diff>
--- a/Resources/DSA_450_LoveBabbar.xlsx
+++ b/Resources/DSA_450_LoveBabbar.xlsx
@@ -1807,7 +1807,7 @@
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -2169,7 +2169,7 @@
       <c r="B31" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="5"/>

</xml_diff>

<commit_message>
done Q27 check if an array is subset of another
</commit_message>
<xml_diff>
--- a/Resources/DSA_450_LoveBabbar.xlsx
+++ b/Resources/DSA_450_LoveBabbar.xlsx
@@ -1804,10 +1804,10 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -2182,7 +2182,7 @@
       <c r="B32" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D32" s="5"/>

</xml_diff>

<commit_message>
completed array DSA questions
</commit_message>
<xml_diff>
--- a/Resources/DSA_450_LoveBabbar.xlsx
+++ b/Resources/DSA_450_LoveBabbar.xlsx
@@ -1711,11 +1711,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1803,11 +1803,11 @@
   </sheetPr>
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -1987,7 +1987,7 @@
       <c r="B17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="5"/>
@@ -2195,7 +2195,7 @@
       <c r="B33" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D33" s="5"/>
@@ -2208,7 +2208,7 @@
       <c r="B34" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="5"/>
@@ -2221,7 +2221,7 @@
       <c r="B35" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D35" s="5"/>
@@ -2234,7 +2234,7 @@
       <c r="B36" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="5"/>
@@ -2247,7 +2247,7 @@
       <c r="B37" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D37" s="5"/>
@@ -2260,7 +2260,7 @@
       <c r="B38" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D38" s="5"/>
@@ -2273,7 +2273,7 @@
       <c r="B39" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="17" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="5"/>
@@ -2286,7 +2286,7 @@
       <c r="B40" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D40" s="5"/>
@@ -2299,7 +2299,7 @@
       <c r="B41" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="16" t="s">
         <v>40</v>
       </c>
       <c r="D41" s="5"/>
@@ -2309,7 +2309,7 @@
         <f aca="false">A41 + 1</f>
         <v>37</v>
       </c>
-      <c r="C42" s="20"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,7 +2318,7 @@
         <v>38</v>
       </c>
       <c r="B43" s="15"/>
-      <c r="C43" s="20"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2329,7 @@
       <c r="B44" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D44" s="5"/>
@@ -2342,7 +2342,7 @@
       <c r="B45" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="20" t="s">
         <v>43</v>
       </c>
       <c r="D45" s="5"/>
@@ -2355,7 +2355,7 @@
       <c r="B46" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="5"/>
@@ -2368,7 +2368,7 @@
       <c r="B47" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D47" s="5"/>
@@ -2381,7 +2381,7 @@
       <c r="B48" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="20" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="5"/>
@@ -2394,7 +2394,7 @@
       <c r="B49" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="5"/>
@@ -2407,7 +2407,7 @@
       <c r="B50" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="20" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="5"/>
@@ -2420,7 +2420,7 @@
       <c r="B51" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="20" t="s">
         <v>49</v>
       </c>
       <c r="D51" s="5"/>
@@ -2433,7 +2433,7 @@
       <c r="B52" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D52" s="5"/>
@@ -2446,7 +2446,7 @@
       <c r="B53" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="20" t="s">
         <v>51</v>
       </c>
       <c r="D53" s="5"/>
@@ -2463,7 +2463,7 @@
         <v>50</v>
       </c>
       <c r="B55" s="15"/>
-      <c r="C55" s="20"/>
+      <c r="C55" s="19"/>
       <c r="D55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2474,7 @@
       <c r="B56" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D56" s="5"/>
@@ -2487,7 +2487,7 @@
       <c r="B57" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="20" t="s">
         <v>54</v>
       </c>
       <c r="D57" s="5"/>
@@ -2500,7 +2500,7 @@
       <c r="B58" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="20" t="s">
         <v>55</v>
       </c>
       <c r="D58" s="5"/>
@@ -2513,7 +2513,7 @@
       <c r="B59" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="19" t="s">
         <v>56</v>
       </c>
       <c r="D59" s="5"/>
@@ -2526,7 +2526,7 @@
       <c r="B60" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D60" s="5"/>
@@ -2539,7 +2539,7 @@
       <c r="B61" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D61" s="5"/>
@@ -2552,7 +2552,7 @@
       <c r="B62" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D62" s="5"/>
@@ -2565,7 +2565,7 @@
       <c r="B63" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D63" s="5"/>
@@ -2578,7 +2578,7 @@
       <c r="B64" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="20" t="s">
         <v>61</v>
       </c>
       <c r="D64" s="5"/>
@@ -2591,7 +2591,7 @@
       <c r="B65" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="20" t="s">
         <v>62</v>
       </c>
       <c r="D65" s="5"/>
@@ -2604,7 +2604,7 @@
       <c r="B66" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="20" t="s">
         <v>63</v>
       </c>
       <c r="D66" s="5"/>
@@ -2617,7 +2617,7 @@
       <c r="B67" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D67" s="5"/>
@@ -2630,7 +2630,7 @@
       <c r="B68" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D68" s="5"/>
@@ -2643,7 +2643,7 @@
       <c r="B69" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D69" s="5"/>
@@ -2656,7 +2656,7 @@
       <c r="B70" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="20" t="s">
         <v>67</v>
       </c>
       <c r="D70" s="5"/>
@@ -2669,7 +2669,7 @@
       <c r="B71" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="20" t="s">
         <v>68</v>
       </c>
       <c r="D71" s="5"/>
@@ -2682,7 +2682,7 @@
       <c r="B72" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="20" t="s">
         <v>69</v>
       </c>
       <c r="D72" s="5"/>
@@ -2695,7 +2695,7 @@
       <c r="B73" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C73" s="20" t="s">
         <v>70</v>
       </c>
       <c r="D73" s="5"/>
@@ -2708,7 +2708,7 @@
       <c r="B74" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C74" s="20" t="s">
         <v>71</v>
       </c>
       <c r="D74" s="5"/>
@@ -2721,7 +2721,7 @@
       <c r="B75" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="20" t="s">
         <v>72</v>
       </c>
       <c r="D75" s="5"/>
@@ -2734,7 +2734,7 @@
       <c r="B76" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" s="20" t="s">
         <v>73</v>
       </c>
       <c r="D76" s="5"/>
@@ -2747,7 +2747,7 @@
       <c r="B77" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" s="20" t="s">
         <v>74</v>
       </c>
       <c r="D77" s="5"/>
@@ -2760,7 +2760,7 @@
       <c r="B78" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C78" s="19" t="s">
+      <c r="C78" s="20" t="s">
         <v>75</v>
       </c>
       <c r="D78" s="5"/>
@@ -2773,7 +2773,7 @@
       <c r="B79" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="C79" s="20" t="s">
         <v>76</v>
       </c>
       <c r="D79" s="5"/>
@@ -2786,7 +2786,7 @@
       <c r="B80" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C80" s="19" t="s">
+      <c r="C80" s="20" t="s">
         <v>77</v>
       </c>
       <c r="D80" s="5"/>
@@ -2799,7 +2799,7 @@
       <c r="B81" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C81" s="20" t="s">
         <v>78</v>
       </c>
       <c r="D81" s="5"/>
@@ -2812,7 +2812,7 @@
       <c r="B82" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="20" t="s">
         <v>79</v>
       </c>
       <c r="D82" s="5"/>
@@ -2825,7 +2825,7 @@
       <c r="B83" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="20" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="5"/>
@@ -2838,7 +2838,7 @@
       <c r="B84" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="20" t="s">
         <v>81</v>
       </c>
       <c r="D84" s="5"/>
@@ -2851,7 +2851,7 @@
       <c r="B85" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="20" t="s">
         <v>82</v>
       </c>
       <c r="D85" s="5"/>
@@ -2864,7 +2864,7 @@
       <c r="B86" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C86" s="19" t="s">
+      <c r="C86" s="20" t="s">
         <v>83</v>
       </c>
       <c r="D86" s="5"/>
@@ -2877,7 +2877,7 @@
       <c r="B87" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="20" t="s">
         <v>84</v>
       </c>
       <c r="D87" s="5"/>
@@ -2890,7 +2890,7 @@
       <c r="B88" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="20" t="s">
         <v>85</v>
       </c>
       <c r="D88" s="5"/>
@@ -2903,7 +2903,7 @@
       <c r="B89" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C89" s="19" t="s">
+      <c r="C89" s="20" t="s">
         <v>86</v>
       </c>
       <c r="D89" s="5"/>
@@ -2916,7 +2916,7 @@
       <c r="B90" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="20" t="s">
         <v>87</v>
       </c>
       <c r="D90" s="5"/>
@@ -2929,7 +2929,7 @@
       <c r="B91" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C91" s="19" t="s">
+      <c r="C91" s="20" t="s">
         <v>88</v>
       </c>
       <c r="D91" s="5"/>
@@ -2942,7 +2942,7 @@
       <c r="B92" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="20" t="s">
         <v>89</v>
       </c>
       <c r="D92" s="5"/>
@@ -2955,7 +2955,7 @@
       <c r="B93" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="20" t="s">
         <v>90</v>
       </c>
       <c r="D93" s="5"/>
@@ -2968,7 +2968,7 @@
       <c r="B94" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D94" s="5"/>
@@ -2981,7 +2981,7 @@
       <c r="B95" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="20" t="s">
         <v>92</v>
       </c>
       <c r="D95" s="5"/>
@@ -2994,7 +2994,7 @@
       <c r="B96" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="20" t="s">
         <v>93</v>
       </c>
       <c r="D96" s="5"/>
@@ -3007,7 +3007,7 @@
       <c r="B97" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="C97" s="20" t="s">
         <v>94</v>
       </c>
       <c r="D97" s="5"/>
@@ -3020,7 +3020,7 @@
       <c r="B98" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="20" t="s">
         <v>95</v>
       </c>
       <c r="D98" s="5"/>
@@ -3037,7 +3037,7 @@
         <v>95</v>
       </c>
       <c r="B100" s="15"/>
-      <c r="C100" s="20"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="5"/>
     </row>
     <row r="101" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3048,7 +3048,7 @@
       <c r="B101" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C101" s="20" t="s">
         <v>97</v>
       </c>
       <c r="D101" s="5"/>
@@ -3061,7 +3061,7 @@
       <c r="B102" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C102" s="19" t="s">
+      <c r="C102" s="20" t="s">
         <v>98</v>
       </c>
       <c r="D102" s="5"/>
@@ -3074,7 +3074,7 @@
       <c r="B103" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="C103" s="20" t="s">
         <v>99</v>
       </c>
       <c r="D103" s="5"/>
@@ -3087,7 +3087,7 @@
       <c r="B104" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="C104" s="20" t="s">
         <v>100</v>
       </c>
       <c r="D104" s="5"/>
@@ -3100,7 +3100,7 @@
       <c r="B105" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C105" s="20" t="s">
         <v>101</v>
       </c>
       <c r="D105" s="5"/>
@@ -3113,7 +3113,7 @@
       <c r="B106" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C106" s="20" t="s">
         <v>102</v>
       </c>
       <c r="D106" s="5"/>
@@ -3126,7 +3126,7 @@
       <c r="B107" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C107" s="19" t="s">
+      <c r="C107" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D107" s="5"/>
@@ -3139,7 +3139,7 @@
       <c r="B108" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C108" s="19" t="s">
+      <c r="C108" s="20" t="s">
         <v>104</v>
       </c>
       <c r="D108" s="5"/>
@@ -3152,7 +3152,7 @@
       <c r="B109" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="C109" s="20" t="s">
         <v>105</v>
       </c>
       <c r="D109" s="5"/>
@@ -3165,7 +3165,7 @@
       <c r="B110" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="20" t="s">
         <v>106</v>
       </c>
       <c r="D110" s="5"/>
@@ -3178,7 +3178,7 @@
       <c r="B111" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C111" s="19" t="s">
+      <c r="C111" s="20" t="s">
         <v>107</v>
       </c>
       <c r="D111" s="5"/>
@@ -3191,7 +3191,7 @@
       <c r="B112" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="C112" s="20" t="s">
         <v>108</v>
       </c>
       <c r="D112" s="5"/>
@@ -3204,7 +3204,7 @@
       <c r="B113" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C113" s="19" t="s">
+      <c r="C113" s="20" t="s">
         <v>109</v>
       </c>
       <c r="D113" s="5"/>
@@ -3217,7 +3217,7 @@
       <c r="B114" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C114" s="19" t="s">
+      <c r="C114" s="20" t="s">
         <v>110</v>
       </c>
       <c r="D114" s="5"/>
@@ -3230,7 +3230,7 @@
       <c r="B115" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="20" t="s">
         <v>111</v>
       </c>
       <c r="D115" s="5"/>
@@ -3243,7 +3243,7 @@
       <c r="B116" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="20" t="s">
         <v>112</v>
       </c>
       <c r="D116" s="5"/>
@@ -3256,7 +3256,7 @@
       <c r="B117" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="20" t="s">
         <v>113</v>
       </c>
       <c r="D117" s="5"/>
@@ -3269,7 +3269,7 @@
       <c r="B118" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C118" s="19" t="s">
+      <c r="C118" s="20" t="s">
         <v>114</v>
       </c>
       <c r="D118" s="5"/>
@@ -3282,7 +3282,7 @@
       <c r="B119" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C119" s="19" t="s">
+      <c r="C119" s="20" t="s">
         <v>115</v>
       </c>
       <c r="D119" s="5"/>
@@ -3295,7 +3295,7 @@
       <c r="B120" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C120" s="19" t="s">
+      <c r="C120" s="20" t="s">
         <v>116</v>
       </c>
       <c r="D120" s="5"/>
@@ -3308,7 +3308,7 @@
       <c r="B121" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C121" s="19" t="s">
+      <c r="C121" s="20" t="s">
         <v>117</v>
       </c>
       <c r="D121" s="5"/>
@@ -3321,7 +3321,7 @@
       <c r="B122" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C122" s="20" t="s">
         <v>118</v>
       </c>
       <c r="D122" s="5"/>
@@ -3334,7 +3334,7 @@
       <c r="B123" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C123" s="20" t="s">
         <v>119</v>
       </c>
       <c r="D123" s="5"/>
@@ -3347,7 +3347,7 @@
       <c r="B124" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C124" s="19" t="s">
+      <c r="C124" s="20" t="s">
         <v>120</v>
       </c>
       <c r="D124" s="5"/>
@@ -3360,7 +3360,7 @@
       <c r="B125" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C125" s="19" t="s">
+      <c r="C125" s="20" t="s">
         <v>121</v>
       </c>
       <c r="D125" s="5"/>
@@ -3373,7 +3373,7 @@
       <c r="B126" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C126" s="19" t="s">
+      <c r="C126" s="20" t="s">
         <v>122</v>
       </c>
       <c r="D126" s="5"/>
@@ -3386,7 +3386,7 @@
       <c r="B127" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C127" s="19" t="s">
+      <c r="C127" s="20" t="s">
         <v>123</v>
       </c>
       <c r="D127" s="5"/>
@@ -3399,7 +3399,7 @@
       <c r="B128" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C128" s="19" t="s">
+      <c r="C128" s="20" t="s">
         <v>124</v>
       </c>
       <c r="D128" s="5"/>
@@ -3412,7 +3412,7 @@
       <c r="B129" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C129" s="19" t="s">
+      <c r="C129" s="20" t="s">
         <v>125</v>
       </c>
       <c r="D129" s="5"/>
@@ -3425,7 +3425,7 @@
       <c r="B130" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C130" s="19" t="s">
+      <c r="C130" s="20" t="s">
         <v>126</v>
       </c>
       <c r="D130" s="5"/>
@@ -3438,7 +3438,7 @@
       <c r="B131" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C131" s="19" t="s">
+      <c r="C131" s="20" t="s">
         <v>127</v>
       </c>
       <c r="D131" s="5"/>
@@ -3451,7 +3451,7 @@
       <c r="B132" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C132" s="19" t="s">
+      <c r="C132" s="20" t="s">
         <v>128</v>
       </c>
       <c r="D132" s="5"/>
@@ -3464,7 +3464,7 @@
       <c r="B133" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C133" s="19" t="s">
+      <c r="C133" s="20" t="s">
         <v>129</v>
       </c>
       <c r="D133" s="5"/>
@@ -3477,7 +3477,7 @@
       <c r="B134" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C134" s="19" t="s">
+      <c r="C134" s="20" t="s">
         <v>130</v>
       </c>
       <c r="D134" s="5"/>
@@ -3490,7 +3490,7 @@
       <c r="B135" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C135" s="19" t="s">
+      <c r="C135" s="20" t="s">
         <v>131</v>
       </c>
       <c r="D135" s="5"/>
@@ -3503,7 +3503,7 @@
       <c r="B136" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C136" s="19" t="s">
+      <c r="C136" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D136" s="5"/>
@@ -3519,7 +3519,7 @@
         <f aca="false">A137 + 1</f>
         <v>133</v>
       </c>
-      <c r="C138" s="20"/>
+      <c r="C138" s="19"/>
       <c r="D138" s="5"/>
     </row>
     <row r="139" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3530,7 +3530,7 @@
       <c r="B139" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C139" s="19" t="s">
+      <c r="C139" s="20" t="s">
         <v>134</v>
       </c>
       <c r="D139" s="5"/>
@@ -3543,7 +3543,7 @@
       <c r="B140" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C140" s="19" t="s">
+      <c r="C140" s="20" t="s">
         <v>135</v>
       </c>
       <c r="D140" s="5"/>
@@ -3556,7 +3556,7 @@
       <c r="B141" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C141" s="19" t="s">
+      <c r="C141" s="20" t="s">
         <v>136</v>
       </c>
       <c r="D141" s="5"/>
@@ -3569,7 +3569,7 @@
       <c r="B142" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C142" s="19" t="s">
+      <c r="C142" s="20" t="s">
         <v>137</v>
       </c>
       <c r="D142" s="5"/>
@@ -3582,7 +3582,7 @@
       <c r="B143" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C143" s="19" t="s">
+      <c r="C143" s="20" t="s">
         <v>138</v>
       </c>
       <c r="D143" s="5"/>
@@ -3595,7 +3595,7 @@
       <c r="B144" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C144" s="19" t="s">
+      <c r="C144" s="20" t="s">
         <v>139</v>
       </c>
       <c r="D144" s="5"/>
@@ -3608,7 +3608,7 @@
       <c r="B145" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C145" s="19" t="s">
+      <c r="C145" s="20" t="s">
         <v>140</v>
       </c>
       <c r="D145" s="5"/>
@@ -3621,7 +3621,7 @@
       <c r="B146" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C146" s="19" t="s">
+      <c r="C146" s="20" t="s">
         <v>141</v>
       </c>
       <c r="D146" s="5"/>
@@ -3634,7 +3634,7 @@
       <c r="B147" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C147" s="19" t="s">
+      <c r="C147" s="20" t="s">
         <v>142</v>
       </c>
       <c r="D147" s="5"/>
@@ -3647,7 +3647,7 @@
       <c r="B148" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C148" s="19" t="s">
+      <c r="C148" s="20" t="s">
         <v>143</v>
       </c>
       <c r="D148" s="5"/>
@@ -3660,7 +3660,7 @@
       <c r="B149" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C149" s="19" t="s">
+      <c r="C149" s="20" t="s">
         <v>144</v>
       </c>
       <c r="D149" s="5"/>
@@ -3673,7 +3673,7 @@
       <c r="B150" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C150" s="19" t="s">
+      <c r="C150" s="20" t="s">
         <v>145</v>
       </c>
       <c r="D150" s="5"/>
@@ -3686,7 +3686,7 @@
       <c r="B151" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C151" s="19" t="s">
+      <c r="C151" s="20" t="s">
         <v>146</v>
       </c>
       <c r="D151" s="5"/>
@@ -3699,7 +3699,7 @@
       <c r="B152" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="19" t="s">
+      <c r="C152" s="20" t="s">
         <v>147</v>
       </c>
       <c r="D152" s="5"/>
@@ -3712,7 +3712,7 @@
       <c r="B153" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C153" s="19" t="s">
+      <c r="C153" s="20" t="s">
         <v>148</v>
       </c>
       <c r="D153" s="5"/>
@@ -3725,7 +3725,7 @@
       <c r="B154" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C154" s="19" t="s">
+      <c r="C154" s="20" t="s">
         <v>149</v>
       </c>
       <c r="D154" s="5"/>
@@ -3738,7 +3738,7 @@
       <c r="B155" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C155" s="19" t="s">
+      <c r="C155" s="20" t="s">
         <v>150</v>
       </c>
       <c r="D155" s="5"/>
@@ -3751,7 +3751,7 @@
       <c r="B156" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C156" s="19" t="s">
+      <c r="C156" s="20" t="s">
         <v>151</v>
       </c>
       <c r="D156" s="5"/>
@@ -3764,7 +3764,7 @@
       <c r="B157" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C157" s="19" t="s">
+      <c r="C157" s="20" t="s">
         <v>152</v>
       </c>
       <c r="D157" s="5"/>
@@ -3777,7 +3777,7 @@
       <c r="B158" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C158" s="19" t="s">
+      <c r="C158" s="20" t="s">
         <v>153</v>
       </c>
       <c r="D158" s="5"/>
@@ -3790,7 +3790,7 @@
       <c r="B159" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C159" s="19" t="s">
+      <c r="C159" s="20" t="s">
         <v>154</v>
       </c>
       <c r="D159" s="5"/>
@@ -3803,7 +3803,7 @@
       <c r="B160" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C160" s="19" t="s">
+      <c r="C160" s="20" t="s">
         <v>155</v>
       </c>
       <c r="D160" s="5"/>
@@ -3816,7 +3816,7 @@
       <c r="B161" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C161" s="19" t="s">
+      <c r="C161" s="20" t="s">
         <v>156</v>
       </c>
       <c r="D161" s="5"/>
@@ -3829,7 +3829,7 @@
       <c r="B162" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C162" s="19" t="s">
+      <c r="C162" s="20" t="s">
         <v>157</v>
       </c>
       <c r="D162" s="5"/>
@@ -3842,7 +3842,7 @@
       <c r="B163" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C163" s="19" t="s">
+      <c r="C163" s="20" t="s">
         <v>158</v>
       </c>
       <c r="D163" s="5"/>
@@ -3855,7 +3855,7 @@
       <c r="B164" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C164" s="20" t="s">
+      <c r="C164" s="19" t="s">
         <v>159</v>
       </c>
       <c r="D164" s="5"/>
@@ -3868,7 +3868,7 @@
       <c r="B165" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C165" s="20" t="s">
+      <c r="C165" s="19" t="s">
         <v>160</v>
       </c>
       <c r="D165" s="5"/>
@@ -3881,7 +3881,7 @@
       <c r="B166" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C166" s="19" t="s">
+      <c r="C166" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D166" s="5"/>
@@ -3894,7 +3894,7 @@
       <c r="B167" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C167" s="19" t="s">
+      <c r="C167" s="20" t="s">
         <v>162</v>
       </c>
       <c r="D167" s="5"/>
@@ -3907,7 +3907,7 @@
       <c r="B168" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C168" s="19" t="s">
+      <c r="C168" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D168" s="5"/>
@@ -3920,7 +3920,7 @@
       <c r="B169" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C169" s="19" t="s">
+      <c r="C169" s="20" t="s">
         <v>164</v>
       </c>
       <c r="D169" s="5"/>
@@ -3933,7 +3933,7 @@
       <c r="B170" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C170" s="19" t="s">
+      <c r="C170" s="20" t="s">
         <v>165</v>
       </c>
       <c r="D170" s="5"/>
@@ -3946,7 +3946,7 @@
       <c r="B171" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C171" s="19" t="s">
+      <c r="C171" s="20" t="s">
         <v>166</v>
       </c>
       <c r="D171" s="5"/>
@@ -3959,7 +3959,7 @@
       <c r="B172" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C172" s="19" t="s">
+      <c r="C172" s="20" t="s">
         <v>167</v>
       </c>
       <c r="D172" s="5"/>
@@ -3972,7 +3972,7 @@
       <c r="B173" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C173" s="19" t="s">
+      <c r="C173" s="20" t="s">
         <v>168</v>
       </c>
       <c r="D173" s="5"/>
@@ -3985,7 +3985,7 @@
       <c r="B174" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C174" s="19" t="s">
+      <c r="C174" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D174" s="5"/>
@@ -4001,7 +4001,7 @@
         <f aca="false">A175 + 1</f>
         <v>171</v>
       </c>
-      <c r="C176" s="20"/>
+      <c r="C176" s="19"/>
       <c r="D176" s="5"/>
     </row>
     <row r="177" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4012,7 +4012,7 @@
       <c r="B177" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C177" s="19" t="s">
+      <c r="C177" s="20" t="s">
         <v>171</v>
       </c>
       <c r="D177" s="5"/>
@@ -4025,7 +4025,7 @@
       <c r="B178" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C178" s="19" t="s">
+      <c r="C178" s="20" t="s">
         <v>172</v>
       </c>
       <c r="D178" s="5"/>
@@ -4038,7 +4038,7 @@
       <c r="B179" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C179" s="19" t="s">
+      <c r="C179" s="20" t="s">
         <v>173</v>
       </c>
       <c r="D179" s="5"/>
@@ -4051,7 +4051,7 @@
       <c r="B180" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C180" s="19" t="s">
+      <c r="C180" s="20" t="s">
         <v>174</v>
       </c>
       <c r="D180" s="5"/>
@@ -4064,7 +4064,7 @@
       <c r="B181" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C181" s="19" t="s">
+      <c r="C181" s="20" t="s">
         <v>175</v>
       </c>
       <c r="D181" s="5"/>
@@ -4077,7 +4077,7 @@
       <c r="B182" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C182" s="19" t="s">
+      <c r="C182" s="20" t="s">
         <v>176</v>
       </c>
       <c r="D182" s="5"/>
@@ -4090,7 +4090,7 @@
       <c r="B183" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C183" s="19" t="s">
+      <c r="C183" s="20" t="s">
         <v>177</v>
       </c>
       <c r="D183" s="5"/>
@@ -4103,7 +4103,7 @@
       <c r="B184" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C184" s="19" t="s">
+      <c r="C184" s="20" t="s">
         <v>178</v>
       </c>
       <c r="D184" s="5"/>
@@ -4116,7 +4116,7 @@
       <c r="B185" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C185" s="19" t="s">
+      <c r="C185" s="20" t="s">
         <v>179</v>
       </c>
       <c r="D185" s="5"/>
@@ -4129,7 +4129,7 @@
       <c r="B186" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C186" s="19" t="s">
+      <c r="C186" s="20" t="s">
         <v>180</v>
       </c>
       <c r="D186" s="5"/>
@@ -4142,7 +4142,7 @@
       <c r="B187" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C187" s="19" t="s">
+      <c r="C187" s="20" t="s">
         <v>181</v>
       </c>
       <c r="D187" s="5"/>
@@ -4155,7 +4155,7 @@
       <c r="B188" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C188" s="19" t="s">
+      <c r="C188" s="20" t="s">
         <v>182</v>
       </c>
       <c r="D188" s="5"/>
@@ -4168,7 +4168,7 @@
       <c r="B189" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C189" s="19" t="s">
+      <c r="C189" s="20" t="s">
         <v>183</v>
       </c>
       <c r="D189" s="5"/>
@@ -4181,7 +4181,7 @@
       <c r="B190" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C190" s="19" t="s">
+      <c r="C190" s="20" t="s">
         <v>184</v>
       </c>
       <c r="D190" s="5"/>
@@ -4194,7 +4194,7 @@
       <c r="B191" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C191" s="19" t="s">
+      <c r="C191" s="20" t="s">
         <v>185</v>
       </c>
       <c r="D191" s="5"/>
@@ -4207,7 +4207,7 @@
       <c r="B192" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C192" s="19" t="s">
+      <c r="C192" s="20" t="s">
         <v>186</v>
       </c>
       <c r="D192" s="5"/>
@@ -4220,7 +4220,7 @@
       <c r="B193" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C193" s="19" t="s">
+      <c r="C193" s="20" t="s">
         <v>187</v>
       </c>
       <c r="D193" s="5"/>
@@ -4233,7 +4233,7 @@
       <c r="B194" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C194" s="19" t="s">
+      <c r="C194" s="20" t="s">
         <v>188</v>
       </c>
       <c r="D194" s="5"/>
@@ -4246,7 +4246,7 @@
       <c r="B195" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C195" s="19" t="s">
+      <c r="C195" s="20" t="s">
         <v>189</v>
       </c>
       <c r="D195" s="5"/>
@@ -4259,7 +4259,7 @@
       <c r="B196" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C196" s="19" t="s">
+      <c r="C196" s="20" t="s">
         <v>190</v>
       </c>
       <c r="D196" s="5"/>
@@ -4272,7 +4272,7 @@
       <c r="B197" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C197" s="19" t="s">
+      <c r="C197" s="20" t="s">
         <v>191</v>
       </c>
       <c r="D197" s="5"/>
@@ -4285,7 +4285,7 @@
       <c r="B198" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C198" s="19" t="s">
+      <c r="C198" s="20" t="s">
         <v>192</v>
       </c>
       <c r="D198" s="5"/>
@@ -4298,7 +4298,7 @@
       <c r="B199" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C199" s="19" t="s">
+      <c r="C199" s="20" t="s">
         <v>193</v>
       </c>
       <c r="D199" s="5"/>
@@ -4311,7 +4311,7 @@
       <c r="B200" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C200" s="19" t="s">
+      <c r="C200" s="20" t="s">
         <v>194</v>
       </c>
       <c r="D200" s="5"/>
@@ -4324,7 +4324,7 @@
       <c r="B201" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C201" s="19" t="s">
+      <c r="C201" s="20" t="s">
         <v>195</v>
       </c>
       <c r="D201" s="5"/>
@@ -4337,7 +4337,7 @@
       <c r="B202" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C202" s="19" t="s">
+      <c r="C202" s="20" t="s">
         <v>196</v>
       </c>
       <c r="D202" s="5"/>
@@ -4350,7 +4350,7 @@
       <c r="B203" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C203" s="19" t="s">
+      <c r="C203" s="20" t="s">
         <v>197</v>
       </c>
       <c r="D203" s="5"/>
@@ -4363,7 +4363,7 @@
       <c r="B204" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C204" s="19" t="s">
+      <c r="C204" s="20" t="s">
         <v>198</v>
       </c>
       <c r="D204" s="5"/>
@@ -4376,7 +4376,7 @@
       <c r="B205" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C205" s="19" t="s">
+      <c r="C205" s="20" t="s">
         <v>199</v>
       </c>
       <c r="D205" s="5"/>
@@ -4389,7 +4389,7 @@
       <c r="B206" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C206" s="19" t="s">
+      <c r="C206" s="20" t="s">
         <v>200</v>
       </c>
       <c r="D206" s="5"/>
@@ -4402,7 +4402,7 @@
       <c r="B207" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C207" s="19" t="s">
+      <c r="C207" s="20" t="s">
         <v>201</v>
       </c>
       <c r="D207" s="5"/>
@@ -4415,7 +4415,7 @@
       <c r="B208" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C208" s="19" t="s">
+      <c r="C208" s="20" t="s">
         <v>202</v>
       </c>
       <c r="D208" s="5"/>
@@ -4428,7 +4428,7 @@
       <c r="B209" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C209" s="19" t="s">
+      <c r="C209" s="20" t="s">
         <v>203</v>
       </c>
       <c r="D209" s="5"/>
@@ -4441,7 +4441,7 @@
       <c r="B210" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C210" s="19" t="s">
+      <c r="C210" s="20" t="s">
         <v>204</v>
       </c>
       <c r="D210" s="5"/>
@@ -4454,7 +4454,7 @@
       <c r="B211" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C211" s="19" t="s">
+      <c r="C211" s="20" t="s">
         <v>205</v>
       </c>
       <c r="D211" s="5"/>
@@ -4465,7 +4465,7 @@
         <v>207</v>
       </c>
       <c r="B212" s="15"/>
-      <c r="C212" s="20"/>
+      <c r="C212" s="19"/>
       <c r="D212" s="5"/>
     </row>
     <row r="213" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4474,7 +4474,7 @@
         <v>208</v>
       </c>
       <c r="B213" s="15"/>
-      <c r="C213" s="20"/>
+      <c r="C213" s="19"/>
       <c r="D213" s="5"/>
     </row>
     <row r="214" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,7 +4485,7 @@
       <c r="B214" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C214" s="19" t="s">
+      <c r="C214" s="20" t="s">
         <v>207</v>
       </c>
       <c r="D214" s="5"/>
@@ -4498,7 +4498,7 @@
       <c r="B215" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C215" s="19" t="s">
+      <c r="C215" s="20" t="s">
         <v>208</v>
       </c>
       <c r="D215" s="5"/>
@@ -4511,7 +4511,7 @@
       <c r="B216" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C216" s="19" t="s">
+      <c r="C216" s="20" t="s">
         <v>209</v>
       </c>
       <c r="D216" s="5"/>
@@ -4524,7 +4524,7 @@
       <c r="B217" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C217" s="19" t="s">
+      <c r="C217" s="20" t="s">
         <v>210</v>
       </c>
       <c r="D217" s="5"/>
@@ -4537,7 +4537,7 @@
       <c r="B218" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C218" s="19" t="s">
+      <c r="C218" s="20" t="s">
         <v>211</v>
       </c>
       <c r="D218" s="5"/>
@@ -4550,7 +4550,7 @@
       <c r="B219" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C219" s="19" t="s">
+      <c r="C219" s="20" t="s">
         <v>212</v>
       </c>
       <c r="D219" s="5"/>
@@ -4576,7 +4576,7 @@
       <c r="B221" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C221" s="19" t="s">
+      <c r="C221" s="20" t="s">
         <v>214</v>
       </c>
       <c r="D221" s="5"/>
@@ -4589,7 +4589,7 @@
       <c r="B222" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C222" s="19" t="s">
+      <c r="C222" s="20" t="s">
         <v>215</v>
       </c>
       <c r="D222" s="5"/>
@@ -4602,7 +4602,7 @@
       <c r="B223" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C223" s="19" t="s">
+      <c r="C223" s="20" t="s">
         <v>216</v>
       </c>
       <c r="D223" s="5"/>
@@ -4615,7 +4615,7 @@
       <c r="B224" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C224" s="19" t="s">
+      <c r="C224" s="20" t="s">
         <v>217</v>
       </c>
       <c r="D224" s="5"/>
@@ -4628,7 +4628,7 @@
       <c r="B225" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C225" s="19" t="s">
+      <c r="C225" s="20" t="s">
         <v>218</v>
       </c>
       <c r="D225" s="5"/>
@@ -4641,7 +4641,7 @@
       <c r="B226" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C226" s="19" t="s">
+      <c r="C226" s="20" t="s">
         <v>219</v>
       </c>
       <c r="D226" s="5"/>
@@ -4654,7 +4654,7 @@
       <c r="B227" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C227" s="19" t="s">
+      <c r="C227" s="20" t="s">
         <v>220</v>
       </c>
       <c r="D227" s="5"/>
@@ -4667,7 +4667,7 @@
       <c r="B228" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C228" s="19" t="s">
+      <c r="C228" s="20" t="s">
         <v>221</v>
       </c>
       <c r="D228" s="5"/>
@@ -4680,7 +4680,7 @@
       <c r="B229" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C229" s="19" t="s">
+      <c r="C229" s="20" t="s">
         <v>222</v>
       </c>
       <c r="D229" s="5"/>
@@ -4693,7 +4693,7 @@
       <c r="B230" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C230" s="19" t="s">
+      <c r="C230" s="20" t="s">
         <v>223</v>
       </c>
       <c r="D230" s="5"/>
@@ -4706,7 +4706,7 @@
       <c r="B231" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C231" s="19" t="s">
+      <c r="C231" s="20" t="s">
         <v>224</v>
       </c>
       <c r="D231" s="5"/>
@@ -4719,7 +4719,7 @@
       <c r="B232" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C232" s="19" t="s">
+      <c r="C232" s="20" t="s">
         <v>225</v>
       </c>
       <c r="D232" s="5"/>
@@ -4732,7 +4732,7 @@
       <c r="B233" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C233" s="19" t="s">
+      <c r="C233" s="20" t="s">
         <v>226</v>
       </c>
       <c r="D233" s="5"/>
@@ -4745,7 +4745,7 @@
       <c r="B234" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C234" s="19" t="s">
+      <c r="C234" s="20" t="s">
         <v>227</v>
       </c>
       <c r="D234" s="5"/>
@@ -4758,7 +4758,7 @@
       <c r="B235" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C235" s="19" t="s">
+      <c r="C235" s="20" t="s">
         <v>228</v>
       </c>
       <c r="D235" s="5"/>
@@ -4768,7 +4768,7 @@
         <f aca="false">A235 + 1</f>
         <v>231</v>
       </c>
-      <c r="C236" s="20"/>
+      <c r="C236" s="19"/>
       <c r="D236" s="5"/>
     </row>
     <row r="237" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4776,7 +4776,7 @@
         <f aca="false">A236 + 1</f>
         <v>232</v>
       </c>
-      <c r="C237" s="20"/>
+      <c r="C237" s="19"/>
       <c r="D237" s="5"/>
     </row>
     <row r="238" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4787,7 +4787,7 @@
       <c r="B238" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C238" s="19" t="s">
+      <c r="C238" s="20" t="s">
         <v>230</v>
       </c>
       <c r="D238" s="5"/>
@@ -4800,7 +4800,7 @@
       <c r="B239" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C239" s="19" t="s">
+      <c r="C239" s="20" t="s">
         <v>231</v>
       </c>
       <c r="D239" s="5"/>
@@ -4813,7 +4813,7 @@
       <c r="B240" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C240" s="19" t="s">
+      <c r="C240" s="20" t="s">
         <v>232</v>
       </c>
       <c r="D240" s="5"/>
@@ -4826,7 +4826,7 @@
       <c r="B241" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C241" s="19" t="s">
+      <c r="C241" s="20" t="s">
         <v>233</v>
       </c>
       <c r="D241" s="5"/>
@@ -4839,7 +4839,7 @@
       <c r="B242" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C242" s="19" t="s">
+      <c r="C242" s="20" t="s">
         <v>234</v>
       </c>
       <c r="D242" s="5"/>
@@ -4852,7 +4852,7 @@
       <c r="B243" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C243" s="19" t="s">
+      <c r="C243" s="20" t="s">
         <v>235</v>
       </c>
       <c r="D243" s="5"/>
@@ -4865,7 +4865,7 @@
       <c r="B244" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C244" s="19" t="s">
+      <c r="C244" s="20" t="s">
         <v>236</v>
       </c>
       <c r="D244" s="5"/>
@@ -4878,7 +4878,7 @@
       <c r="B245" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C245" s="19" t="s">
+      <c r="C245" s="20" t="s">
         <v>237</v>
       </c>
       <c r="D245" s="5"/>
@@ -4891,7 +4891,7 @@
       <c r="B246" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C246" s="19" t="s">
+      <c r="C246" s="20" t="s">
         <v>238</v>
       </c>
       <c r="D246" s="5"/>
@@ -4904,7 +4904,7 @@
       <c r="B247" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C247" s="19" t="s">
+      <c r="C247" s="20" t="s">
         <v>239</v>
       </c>
       <c r="D247" s="5"/>
@@ -4917,7 +4917,7 @@
       <c r="B248" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C248" s="19" t="s">
+      <c r="C248" s="20" t="s">
         <v>240</v>
       </c>
       <c r="D248" s="5"/>
@@ -4930,7 +4930,7 @@
       <c r="B249" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C249" s="19" t="s">
+      <c r="C249" s="20" t="s">
         <v>241</v>
       </c>
       <c r="D249" s="5"/>
@@ -4943,7 +4943,7 @@
       <c r="B250" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C250" s="19" t="s">
+      <c r="C250" s="20" t="s">
         <v>242</v>
       </c>
       <c r="D250" s="5"/>
@@ -4956,7 +4956,7 @@
       <c r="B251" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C251" s="19" t="s">
+      <c r="C251" s="20" t="s">
         <v>243</v>
       </c>
       <c r="D251" s="5"/>
@@ -4969,7 +4969,7 @@
       <c r="B252" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C252" s="19" t="s">
+      <c r="C252" s="20" t="s">
         <v>244</v>
       </c>
       <c r="D252" s="5"/>
@@ -4982,7 +4982,7 @@
       <c r="B253" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C253" s="19" t="s">
+      <c r="C253" s="20" t="s">
         <v>245</v>
       </c>
       <c r="D253" s="5"/>
@@ -4995,7 +4995,7 @@
       <c r="B254" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C254" s="19" t="s">
+      <c r="C254" s="20" t="s">
         <v>246</v>
       </c>
       <c r="D254" s="5"/>
@@ -5008,7 +5008,7 @@
       <c r="B255" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C255" s="19" t="s">
+      <c r="C255" s="20" t="s">
         <v>247</v>
       </c>
       <c r="D255" s="5"/>
@@ -5021,7 +5021,7 @@
       <c r="B256" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C256" s="19" t="s">
+      <c r="C256" s="20" t="s">
         <v>248</v>
       </c>
       <c r="D256" s="5"/>
@@ -5034,7 +5034,7 @@
       <c r="B257" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C257" s="19" t="s">
+      <c r="C257" s="20" t="s">
         <v>249</v>
       </c>
       <c r="D257" s="5"/>
@@ -5047,7 +5047,7 @@
       <c r="B258" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C258" s="19" t="s">
+      <c r="C258" s="20" t="s">
         <v>250</v>
       </c>
       <c r="D258" s="5"/>
@@ -5060,7 +5060,7 @@
       <c r="B259" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C259" s="19" t="s">
+      <c r="C259" s="20" t="s">
         <v>251</v>
       </c>
       <c r="D259" s="5"/>
@@ -5073,7 +5073,7 @@
       <c r="B260" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C260" s="19" t="s">
+      <c r="C260" s="20" t="s">
         <v>252</v>
       </c>
       <c r="D260" s="5"/>
@@ -5086,7 +5086,7 @@
       <c r="B261" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C261" s="19" t="s">
+      <c r="C261" s="20" t="s">
         <v>253</v>
       </c>
       <c r="D261" s="5"/>
@@ -5099,7 +5099,7 @@
       <c r="B262" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C262" s="19" t="s">
+      <c r="C262" s="20" t="s">
         <v>254</v>
       </c>
       <c r="D262" s="5"/>
@@ -5112,7 +5112,7 @@
       <c r="B263" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C263" s="19" t="s">
+      <c r="C263" s="20" t="s">
         <v>255</v>
       </c>
       <c r="D263" s="5"/>
@@ -5125,7 +5125,7 @@
       <c r="B264" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C264" s="19" t="s">
+      <c r="C264" s="20" t="s">
         <v>256</v>
       </c>
       <c r="D264" s="5"/>
@@ -5138,7 +5138,7 @@
       <c r="B265" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C265" s="19" t="s">
+      <c r="C265" s="20" t="s">
         <v>257</v>
       </c>
       <c r="D265" s="5"/>
@@ -5151,7 +5151,7 @@
       <c r="B266" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C266" s="19" t="s">
+      <c r="C266" s="20" t="s">
         <v>258</v>
       </c>
       <c r="D266" s="5"/>
@@ -5164,7 +5164,7 @@
       <c r="B267" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C267" s="19" t="s">
+      <c r="C267" s="20" t="s">
         <v>259</v>
       </c>
       <c r="D267" s="5"/>
@@ -5177,7 +5177,7 @@
       <c r="B268" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C268" s="19" t="s">
+      <c r="C268" s="20" t="s">
         <v>260</v>
       </c>
       <c r="D268" s="5"/>
@@ -5190,7 +5190,7 @@
       <c r="B269" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C269" s="19" t="s">
+      <c r="C269" s="20" t="s">
         <v>261</v>
       </c>
       <c r="D269" s="5"/>
@@ -5203,7 +5203,7 @@
       <c r="B270" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C270" s="19" t="s">
+      <c r="C270" s="20" t="s">
         <v>262</v>
       </c>
       <c r="D270" s="5"/>
@@ -5216,7 +5216,7 @@
       <c r="B271" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C271" s="19" t="s">
+      <c r="C271" s="20" t="s">
         <v>86</v>
       </c>
       <c r="D271" s="5"/>
@@ -5229,7 +5229,7 @@
       <c r="B272" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="C272" s="19" t="s">
+      <c r="C272" s="20" t="s">
         <v>263</v>
       </c>
       <c r="D272" s="5"/>
@@ -5239,7 +5239,7 @@
         <f aca="false">A272 + 1</f>
         <v>268</v>
       </c>
-      <c r="C273" s="20"/>
+      <c r="C273" s="19"/>
       <c r="D273" s="5"/>
     </row>
     <row r="274" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5247,7 +5247,7 @@
         <f aca="false">A273 + 1</f>
         <v>269</v>
       </c>
-      <c r="C274" s="20"/>
+      <c r="C274" s="19"/>
       <c r="D274" s="5"/>
     </row>
     <row r="275" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5258,7 +5258,7 @@
       <c r="B275" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C275" s="19" t="s">
+      <c r="C275" s="20" t="s">
         <v>265</v>
       </c>
       <c r="D275" s="5"/>
@@ -5271,7 +5271,7 @@
       <c r="B276" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C276" s="19" t="s">
+      <c r="C276" s="20" t="s">
         <v>266</v>
       </c>
       <c r="D276" s="5"/>
@@ -5284,7 +5284,7 @@
       <c r="B277" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C277" s="19" t="s">
+      <c r="C277" s="20" t="s">
         <v>267</v>
       </c>
       <c r="D277" s="5"/>
@@ -5297,7 +5297,7 @@
       <c r="B278" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C278" s="19" t="s">
+      <c r="C278" s="20" t="s">
         <v>268</v>
       </c>
       <c r="D278" s="5"/>
@@ -5310,7 +5310,7 @@
       <c r="B279" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C279" s="19" t="s">
+      <c r="C279" s="20" t="s">
         <v>269</v>
       </c>
       <c r="D279" s="5"/>
@@ -5323,7 +5323,7 @@
       <c r="B280" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C280" s="19" t="s">
+      <c r="C280" s="20" t="s">
         <v>270</v>
       </c>
       <c r="D280" s="5"/>
@@ -5336,7 +5336,7 @@
       <c r="B281" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C281" s="19" t="s">
+      <c r="C281" s="20" t="s">
         <v>271</v>
       </c>
       <c r="D281" s="5"/>
@@ -5349,7 +5349,7 @@
       <c r="B282" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C282" s="19" t="s">
+      <c r="C282" s="20" t="s">
         <v>272</v>
       </c>
       <c r="D282" s="5"/>
@@ -5362,7 +5362,7 @@
       <c r="B283" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C283" s="19" t="s">
+      <c r="C283" s="20" t="s">
         <v>273</v>
       </c>
       <c r="D283" s="5"/>
@@ -5375,7 +5375,7 @@
       <c r="B284" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C284" s="19" t="s">
+      <c r="C284" s="20" t="s">
         <v>274</v>
       </c>
       <c r="D284" s="5"/>
@@ -5388,7 +5388,7 @@
       <c r="B285" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C285" s="19" t="s">
+      <c r="C285" s="20" t="s">
         <v>275</v>
       </c>
       <c r="D285" s="5"/>
@@ -5401,7 +5401,7 @@
       <c r="B286" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C286" s="19" t="s">
+      <c r="C286" s="20" t="s">
         <v>276</v>
       </c>
       <c r="D286" s="5"/>
@@ -5414,7 +5414,7 @@
       <c r="B287" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C287" s="19" t="s">
+      <c r="C287" s="20" t="s">
         <v>277</v>
       </c>
       <c r="D287" s="5"/>
@@ -5427,7 +5427,7 @@
       <c r="B288" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C288" s="19" t="s">
+      <c r="C288" s="20" t="s">
         <v>278</v>
       </c>
       <c r="D288" s="5"/>
@@ -5440,7 +5440,7 @@
       <c r="B289" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C289" s="19" t="s">
+      <c r="C289" s="20" t="s">
         <v>279</v>
       </c>
       <c r="D289" s="5"/>
@@ -5453,7 +5453,7 @@
       <c r="B290" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C290" s="19" t="s">
+      <c r="C290" s="20" t="s">
         <v>280</v>
       </c>
       <c r="D290" s="5"/>
@@ -5466,7 +5466,7 @@
       <c r="B291" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C291" s="19" t="s">
+      <c r="C291" s="20" t="s">
         <v>281</v>
       </c>
       <c r="D291" s="5"/>
@@ -5479,7 +5479,7 @@
       <c r="B292" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C292" s="19" t="s">
+      <c r="C292" s="20" t="s">
         <v>282</v>
       </c>
       <c r="D292" s="5"/>
@@ -5492,7 +5492,7 @@
       <c r="B293" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C293" s="19" t="s">
+      <c r="C293" s="20" t="s">
         <v>283</v>
       </c>
       <c r="D293" s="5"/>
@@ -5502,7 +5502,7 @@
         <f aca="false">A293 + 1</f>
         <v>289</v>
       </c>
-      <c r="C294" s="20"/>
+      <c r="C294" s="19"/>
       <c r="D294" s="5"/>
     </row>
     <row r="295" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5510,7 +5510,7 @@
         <f aca="false">A294 + 1</f>
         <v>290</v>
       </c>
-      <c r="C295" s="20"/>
+      <c r="C295" s="19"/>
       <c r="D295" s="5"/>
     </row>
     <row r="296" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5521,7 +5521,7 @@
       <c r="B296" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C296" s="19" t="s">
+      <c r="C296" s="20" t="s">
         <v>285</v>
       </c>
       <c r="D296" s="5"/>
@@ -5534,7 +5534,7 @@
       <c r="B297" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C297" s="19" t="s">
+      <c r="C297" s="20" t="s">
         <v>286</v>
       </c>
       <c r="D297" s="5"/>
@@ -5547,7 +5547,7 @@
       <c r="B298" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C298" s="19" t="s">
+      <c r="C298" s="20" t="s">
         <v>287</v>
       </c>
       <c r="D298" s="5"/>
@@ -5560,7 +5560,7 @@
       <c r="B299" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C299" s="19" t="s">
+      <c r="C299" s="20" t="s">
         <v>288</v>
       </c>
       <c r="D299" s="5"/>
@@ -5573,7 +5573,7 @@
       <c r="B300" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C300" s="19" t="s">
+      <c r="C300" s="20" t="s">
         <v>289</v>
       </c>
       <c r="D300" s="5"/>
@@ -5586,7 +5586,7 @@
       <c r="B301" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C301" s="19" t="s">
+      <c r="C301" s="20" t="s">
         <v>290</v>
       </c>
       <c r="D301" s="5"/>
@@ -5599,7 +5599,7 @@
       <c r="B302" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C302" s="19" t="s">
+      <c r="C302" s="20" t="s">
         <v>291</v>
       </c>
       <c r="D302" s="5"/>
@@ -5612,7 +5612,7 @@
       <c r="B303" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C303" s="19" t="s">
+      <c r="C303" s="20" t="s">
         <v>292</v>
       </c>
       <c r="D303" s="5"/>
@@ -5625,7 +5625,7 @@
       <c r="B304" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C304" s="19" t="s">
+      <c r="C304" s="20" t="s">
         <v>293</v>
       </c>
       <c r="D304" s="5"/>
@@ -5638,7 +5638,7 @@
       <c r="B305" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C305" s="19" t="s">
+      <c r="C305" s="20" t="s">
         <v>294</v>
       </c>
       <c r="D305" s="5"/>
@@ -5651,7 +5651,7 @@
       <c r="B306" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C306" s="19" t="s">
+      <c r="C306" s="20" t="s">
         <v>295</v>
       </c>
       <c r="D306" s="5"/>
@@ -5664,7 +5664,7 @@
       <c r="B307" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C307" s="19" t="s">
+      <c r="C307" s="20" t="s">
         <v>296</v>
       </c>
       <c r="D307" s="5"/>
@@ -5677,7 +5677,7 @@
       <c r="B308" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C308" s="19" t="s">
+      <c r="C308" s="20" t="s">
         <v>297</v>
       </c>
       <c r="D308" s="5"/>
@@ -5703,7 +5703,7 @@
       <c r="B310" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C310" s="19" t="s">
+      <c r="C310" s="20" t="s">
         <v>299</v>
       </c>
       <c r="D310" s="5"/>
@@ -5716,7 +5716,7 @@
       <c r="B311" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C311" s="19" t="s">
+      <c r="C311" s="20" t="s">
         <v>300</v>
       </c>
       <c r="D311" s="5"/>
@@ -5729,7 +5729,7 @@
       <c r="B312" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C312" s="19" t="s">
+      <c r="C312" s="20" t="s">
         <v>301</v>
       </c>
       <c r="D312" s="5"/>
@@ -5742,7 +5742,7 @@
       <c r="B313" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C313" s="19" t="s">
+      <c r="C313" s="20" t="s">
         <v>302</v>
       </c>
       <c r="D313" s="5"/>
@@ -5755,7 +5755,7 @@
       <c r="B314" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C314" s="19" t="s">
+      <c r="C314" s="20" t="s">
         <v>303</v>
       </c>
       <c r="D314" s="5"/>
@@ -5768,7 +5768,7 @@
       <c r="B315" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C315" s="19" t="s">
+      <c r="C315" s="20" t="s">
         <v>304</v>
       </c>
       <c r="D315" s="5"/>
@@ -5781,7 +5781,7 @@
       <c r="B316" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C316" s="19" t="s">
+      <c r="C316" s="20" t="s">
         <v>305</v>
       </c>
       <c r="D316" s="5"/>
@@ -5794,7 +5794,7 @@
       <c r="B317" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C317" s="19" t="s">
+      <c r="C317" s="20" t="s">
         <v>306</v>
       </c>
       <c r="D317" s="5"/>
@@ -5807,7 +5807,7 @@
       <c r="B318" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C318" s="19" t="s">
+      <c r="C318" s="20" t="s">
         <v>307</v>
       </c>
       <c r="D318" s="5"/>
@@ -5820,7 +5820,7 @@
       <c r="B319" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C319" s="19" t="s">
+      <c r="C319" s="20" t="s">
         <v>308</v>
       </c>
       <c r="D319" s="5"/>
@@ -5833,7 +5833,7 @@
       <c r="B320" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C320" s="19" t="s">
+      <c r="C320" s="20" t="s">
         <v>309</v>
       </c>
       <c r="D320" s="5"/>
@@ -5846,7 +5846,7 @@
       <c r="B321" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C321" s="19" t="s">
+      <c r="C321" s="20" t="s">
         <v>310</v>
       </c>
       <c r="D321" s="5"/>
@@ -5859,7 +5859,7 @@
       <c r="B322" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C322" s="19" t="s">
+      <c r="C322" s="20" t="s">
         <v>311</v>
       </c>
       <c r="D322" s="5"/>
@@ -5872,7 +5872,7 @@
       <c r="B323" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C323" s="19" t="s">
+      <c r="C323" s="20" t="s">
         <v>312</v>
       </c>
       <c r="D323" s="5"/>
@@ -5885,7 +5885,7 @@
       <c r="B324" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C324" s="19" t="s">
+      <c r="C324" s="20" t="s">
         <v>313</v>
       </c>
       <c r="D324" s="5"/>
@@ -5898,7 +5898,7 @@
       <c r="B325" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C325" s="19" t="s">
+      <c r="C325" s="20" t="s">
         <v>314</v>
       </c>
       <c r="D325" s="5"/>
@@ -5911,7 +5911,7 @@
       <c r="B326" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C326" s="19" t="s">
+      <c r="C326" s="20" t="s">
         <v>315</v>
       </c>
       <c r="D326" s="5"/>
@@ -5924,7 +5924,7 @@
       <c r="B327" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C327" s="19" t="s">
+      <c r="C327" s="20" t="s">
         <v>316</v>
       </c>
       <c r="D327" s="5"/>
@@ -5937,7 +5937,7 @@
       <c r="B328" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C328" s="19" t="s">
+      <c r="C328" s="20" t="s">
         <v>317</v>
       </c>
       <c r="D328" s="5"/>
@@ -5950,7 +5950,7 @@
       <c r="B329" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C329" s="19" t="s">
+      <c r="C329" s="20" t="s">
         <v>318</v>
       </c>
       <c r="D329" s="5"/>
@@ -5963,7 +5963,7 @@
       <c r="B330" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C330" s="19" t="s">
+      <c r="C330" s="20" t="s">
         <v>319</v>
       </c>
       <c r="D330" s="5"/>
@@ -5976,7 +5976,7 @@
       <c r="B331" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C331" s="19" t="s">
+      <c r="C331" s="20" t="s">
         <v>320</v>
       </c>
       <c r="D331" s="5"/>
@@ -5989,7 +5989,7 @@
       <c r="B332" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C332" s="19" t="s">
+      <c r="C332" s="20" t="s">
         <v>321</v>
       </c>
       <c r="D332" s="5"/>
@@ -6002,7 +6002,7 @@
       <c r="B333" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C333" s="19" t="s">
+      <c r="C333" s="20" t="s">
         <v>322</v>
       </c>
       <c r="D333" s="5"/>
@@ -6012,7 +6012,7 @@
         <f aca="false">A333 + 1</f>
         <v>329</v>
       </c>
-      <c r="C334" s="20"/>
+      <c r="C334" s="19"/>
       <c r="D334" s="5"/>
     </row>
     <row r="335" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6020,7 +6020,7 @@
         <f aca="false">A334 + 1</f>
         <v>330</v>
       </c>
-      <c r="C335" s="20"/>
+      <c r="C335" s="19"/>
       <c r="D335" s="5"/>
     </row>
     <row r="336" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6031,7 +6031,7 @@
       <c r="B336" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C336" s="19" t="s">
+      <c r="C336" s="20" t="s">
         <v>324</v>
       </c>
       <c r="D336" s="5"/>
@@ -6044,7 +6044,7 @@
       <c r="B337" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C337" s="19" t="s">
+      <c r="C337" s="20" t="s">
         <v>325</v>
       </c>
       <c r="D337" s="5"/>
@@ -6057,7 +6057,7 @@
       <c r="B338" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C338" s="19" t="s">
+      <c r="C338" s="20" t="s">
         <v>326</v>
       </c>
       <c r="D338" s="5"/>
@@ -6070,7 +6070,7 @@
       <c r="B339" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C339" s="19" t="s">
+      <c r="C339" s="20" t="s">
         <v>327</v>
       </c>
       <c r="D339" s="5"/>
@@ -6083,7 +6083,7 @@
       <c r="B340" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C340" s="19" t="s">
+      <c r="C340" s="20" t="s">
         <v>328</v>
       </c>
       <c r="D340" s="5"/>
@@ -6096,7 +6096,7 @@
       <c r="B341" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C341" s="19" t="s">
+      <c r="C341" s="20" t="s">
         <v>329</v>
       </c>
       <c r="D341" s="5"/>
@@ -6109,7 +6109,7 @@
       <c r="B342" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C342" s="19" t="s">
+      <c r="C342" s="20" t="s">
         <v>330</v>
       </c>
       <c r="D342" s="5"/>
@@ -6122,7 +6122,7 @@
       <c r="B343" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C343" s="19" t="s">
+      <c r="C343" s="20" t="s">
         <v>331</v>
       </c>
       <c r="D343" s="5"/>
@@ -6148,7 +6148,7 @@
       <c r="B345" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C345" s="19" t="s">
+      <c r="C345" s="20" t="s">
         <v>333</v>
       </c>
       <c r="D345" s="5"/>
@@ -6161,7 +6161,7 @@
       <c r="B346" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C346" s="19" t="s">
+      <c r="C346" s="20" t="s">
         <v>334</v>
       </c>
       <c r="D346" s="5"/>
@@ -6174,7 +6174,7 @@
       <c r="B347" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C347" s="19" t="s">
+      <c r="C347" s="20" t="s">
         <v>335</v>
       </c>
       <c r="D347" s="5"/>
@@ -6187,7 +6187,7 @@
       <c r="B348" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C348" s="19" t="s">
+      <c r="C348" s="20" t="s">
         <v>336</v>
       </c>
       <c r="D348" s="5"/>
@@ -6200,7 +6200,7 @@
       <c r="B349" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C349" s="19" t="s">
+      <c r="C349" s="20" t="s">
         <v>337</v>
       </c>
       <c r="D349" s="5"/>
@@ -6213,7 +6213,7 @@
       <c r="B350" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C350" s="19" t="s">
+      <c r="C350" s="20" t="s">
         <v>338</v>
       </c>
       <c r="D350" s="5"/>
@@ -6226,7 +6226,7 @@
       <c r="B351" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C351" s="19" t="s">
+      <c r="C351" s="20" t="s">
         <v>339</v>
       </c>
       <c r="D351" s="5"/>
@@ -6239,7 +6239,7 @@
       <c r="B352" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C352" s="19" t="s">
+      <c r="C352" s="20" t="s">
         <v>340</v>
       </c>
       <c r="D352" s="5"/>
@@ -6252,7 +6252,7 @@
       <c r="B353" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C353" s="19" t="s">
+      <c r="C353" s="20" t="s">
         <v>341</v>
       </c>
       <c r="D353" s="5"/>
@@ -6262,7 +6262,7 @@
         <f aca="false">A353 + 1</f>
         <v>349</v>
       </c>
-      <c r="C354" s="20"/>
+      <c r="C354" s="19"/>
       <c r="D354" s="5"/>
     </row>
     <row r="355" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,7 +6270,7 @@
         <f aca="false">A354 + 1</f>
         <v>350</v>
       </c>
-      <c r="C355" s="20"/>
+      <c r="C355" s="19"/>
       <c r="D355" s="5"/>
     </row>
     <row r="356" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6281,7 +6281,7 @@
       <c r="B356" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C356" s="19" t="s">
+      <c r="C356" s="20" t="s">
         <v>343</v>
       </c>
       <c r="D356" s="5"/>
@@ -6294,7 +6294,7 @@
       <c r="B357" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C357" s="19" t="s">
+      <c r="C357" s="20" t="s">
         <v>344</v>
       </c>
       <c r="D357" s="5"/>
@@ -6307,7 +6307,7 @@
       <c r="B358" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C358" s="19" t="s">
+      <c r="C358" s="20" t="s">
         <v>345</v>
       </c>
       <c r="D358" s="5"/>
@@ -6320,7 +6320,7 @@
       <c r="B359" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C359" s="19" t="s">
+      <c r="C359" s="20" t="s">
         <v>346</v>
       </c>
       <c r="D359" s="5"/>
@@ -6333,7 +6333,7 @@
       <c r="B360" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C360" s="19" t="s">
+      <c r="C360" s="20" t="s">
         <v>347</v>
       </c>
       <c r="D360" s="5"/>
@@ -6346,7 +6346,7 @@
       <c r="B361" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C361" s="19" t="s">
+      <c r="C361" s="20" t="s">
         <v>348</v>
       </c>
       <c r="D361" s="5"/>
@@ -6359,7 +6359,7 @@
       <c r="B362" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C362" s="19" t="s">
+      <c r="C362" s="20" t="s">
         <v>349</v>
       </c>
       <c r="D362" s="5"/>
@@ -6372,7 +6372,7 @@
       <c r="B363" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C363" s="19" t="s">
+      <c r="C363" s="20" t="s">
         <v>350</v>
       </c>
       <c r="D363" s="5"/>
@@ -6385,7 +6385,7 @@
       <c r="B364" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C364" s="19" t="s">
+      <c r="C364" s="20" t="s">
         <v>351</v>
       </c>
       <c r="D364" s="5"/>
@@ -6398,7 +6398,7 @@
       <c r="B365" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C365" s="19" t="s">
+      <c r="C365" s="20" t="s">
         <v>352</v>
       </c>
       <c r="D365" s="5"/>
@@ -6411,7 +6411,7 @@
       <c r="B366" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C366" s="19" t="s">
+      <c r="C366" s="20" t="s">
         <v>353</v>
       </c>
       <c r="D366" s="5"/>
@@ -6424,7 +6424,7 @@
       <c r="B367" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C367" s="19" t="s">
+      <c r="C367" s="20" t="s">
         <v>354</v>
       </c>
       <c r="D367" s="5"/>
@@ -6437,7 +6437,7 @@
       <c r="B368" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C368" s="19" t="s">
+      <c r="C368" s="20" t="s">
         <v>355</v>
       </c>
       <c r="D368" s="5"/>
@@ -6450,7 +6450,7 @@
       <c r="B369" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C369" s="19" t="s">
+      <c r="C369" s="20" t="s">
         <v>356</v>
       </c>
       <c r="D369" s="5"/>
@@ -6463,7 +6463,7 @@
       <c r="B370" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C370" s="19" t="s">
+      <c r="C370" s="20" t="s">
         <v>357</v>
       </c>
       <c r="D370" s="5"/>
@@ -6476,7 +6476,7 @@
       <c r="B371" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C371" s="19" t="s">
+      <c r="C371" s="20" t="s">
         <v>358</v>
       </c>
       <c r="D371" s="5"/>
@@ -6489,7 +6489,7 @@
       <c r="B372" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C372" s="19" t="s">
+      <c r="C372" s="20" t="s">
         <v>359</v>
       </c>
       <c r="D372" s="5"/>
@@ -6502,7 +6502,7 @@
       <c r="B373" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C373" s="19" t="s">
+      <c r="C373" s="20" t="s">
         <v>360</v>
       </c>
       <c r="D373" s="5"/>
@@ -6515,7 +6515,7 @@
       <c r="B374" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C374" s="19" t="s">
+      <c r="C374" s="20" t="s">
         <v>361</v>
       </c>
       <c r="D374" s="5"/>
@@ -6528,7 +6528,7 @@
       <c r="B375" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C375" s="19" t="s">
+      <c r="C375" s="20" t="s">
         <v>362</v>
       </c>
       <c r="D375" s="5"/>
@@ -6541,7 +6541,7 @@
       <c r="B376" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C376" s="19" t="s">
+      <c r="C376" s="20" t="s">
         <v>363</v>
       </c>
       <c r="D376" s="5"/>
@@ -6554,7 +6554,7 @@
       <c r="B377" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C377" s="19" t="s">
+      <c r="C377" s="20" t="s">
         <v>364</v>
       </c>
       <c r="D377" s="5"/>
@@ -6567,7 +6567,7 @@
       <c r="B378" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C378" s="19" t="s">
+      <c r="C378" s="20" t="s">
         <v>365</v>
       </c>
       <c r="D378" s="5"/>
@@ -6580,7 +6580,7 @@
       <c r="B379" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C379" s="19" t="s">
+      <c r="C379" s="20" t="s">
         <v>366</v>
       </c>
       <c r="D379" s="5"/>
@@ -6593,7 +6593,7 @@
       <c r="B380" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C380" s="19" t="s">
+      <c r="C380" s="20" t="s">
         <v>367</v>
       </c>
       <c r="D380" s="5"/>
@@ -6606,7 +6606,7 @@
       <c r="B381" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C381" s="19" t="s">
+      <c r="C381" s="20" t="s">
         <v>368</v>
       </c>
       <c r="D381" s="5"/>
@@ -6619,7 +6619,7 @@
       <c r="B382" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C382" s="19" t="s">
+      <c r="C382" s="20" t="s">
         <v>369</v>
       </c>
       <c r="D382" s="5"/>
@@ -6632,7 +6632,7 @@
       <c r="B383" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C383" s="19" t="s">
+      <c r="C383" s="20" t="s">
         <v>370</v>
       </c>
       <c r="D383" s="5"/>
@@ -6645,7 +6645,7 @@
       <c r="B384" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C384" s="19" t="s">
+      <c r="C384" s="20" t="s">
         <v>371</v>
       </c>
       <c r="D384" s="5"/>
@@ -6658,7 +6658,7 @@
       <c r="B385" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C385" s="19" t="s">
+      <c r="C385" s="20" t="s">
         <v>372</v>
       </c>
       <c r="D385" s="5"/>
@@ -6671,7 +6671,7 @@
       <c r="B386" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C386" s="19" t="s">
+      <c r="C386" s="20" t="s">
         <v>373</v>
       </c>
       <c r="D386" s="5"/>
@@ -6684,7 +6684,7 @@
       <c r="B387" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C387" s="19" t="s">
+      <c r="C387" s="20" t="s">
         <v>374</v>
       </c>
       <c r="D387" s="5"/>
@@ -6697,7 +6697,7 @@
       <c r="B388" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C388" s="19" t="s">
+      <c r="C388" s="20" t="s">
         <v>375</v>
       </c>
       <c r="D388" s="5"/>
@@ -6710,7 +6710,7 @@
       <c r="B389" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C389" s="19" t="s">
+      <c r="C389" s="20" t="s">
         <v>376</v>
       </c>
       <c r="D389" s="5"/>
@@ -6723,7 +6723,7 @@
       <c r="B390" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C390" s="19" t="s">
+      <c r="C390" s="20" t="s">
         <v>376</v>
       </c>
       <c r="D390" s="5"/>
@@ -6736,7 +6736,7 @@
       <c r="B391" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C391" s="19" t="s">
+      <c r="C391" s="20" t="s">
         <v>377</v>
       </c>
       <c r="D391" s="5"/>
@@ -6749,7 +6749,7 @@
       <c r="B392" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C392" s="19" t="s">
+      <c r="C392" s="20" t="s">
         <v>378</v>
       </c>
       <c r="D392" s="5"/>
@@ -6762,7 +6762,7 @@
       <c r="B393" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C393" s="19" t="s">
+      <c r="C393" s="20" t="s">
         <v>379</v>
       </c>
       <c r="D393" s="5"/>
@@ -6775,7 +6775,7 @@
       <c r="B394" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C394" s="19" t="s">
+      <c r="C394" s="20" t="s">
         <v>380</v>
       </c>
       <c r="D394" s="5"/>
@@ -6788,7 +6788,7 @@
       <c r="B395" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C395" s="19" t="s">
+      <c r="C395" s="20" t="s">
         <v>381</v>
       </c>
       <c r="D395" s="5"/>
@@ -6801,7 +6801,7 @@
       <c r="B396" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C396" s="19" t="s">
+      <c r="C396" s="20" t="s">
         <v>382</v>
       </c>
       <c r="D396" s="5"/>
@@ -6814,7 +6814,7 @@
       <c r="B397" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C397" s="19" t="s">
+      <c r="C397" s="20" t="s">
         <v>383</v>
       </c>
       <c r="D397" s="5"/>
@@ -6827,7 +6827,7 @@
       <c r="B398" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C398" s="19" t="s">
+      <c r="C398" s="20" t="s">
         <v>384</v>
       </c>
       <c r="D398" s="5"/>
@@ -6840,7 +6840,7 @@
       <c r="B399" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="C399" s="19" t="s">
+      <c r="C399" s="20" t="s">
         <v>385</v>
       </c>
       <c r="D399" s="5"/>
@@ -6850,7 +6850,7 @@
         <f aca="false">A399 + 1</f>
         <v>395</v>
       </c>
-      <c r="C400" s="20"/>
+      <c r="C400" s="19"/>
       <c r="D400" s="5"/>
     </row>
     <row r="401" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6858,7 +6858,7 @@
         <f aca="false">A400 + 1</f>
         <v>396</v>
       </c>
-      <c r="C401" s="20"/>
+      <c r="C401" s="19"/>
       <c r="D401" s="5"/>
     </row>
     <row r="402" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,7 +6869,7 @@
       <c r="B402" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C402" s="19" t="s">
+      <c r="C402" s="20" t="s">
         <v>387</v>
       </c>
       <c r="D402" s="5"/>
@@ -6882,7 +6882,7 @@
       <c r="B403" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C403" s="19" t="s">
+      <c r="C403" s="20" t="s">
         <v>388</v>
       </c>
       <c r="D403" s="5"/>
@@ -6895,7 +6895,7 @@
       <c r="B404" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C404" s="19" t="s">
+      <c r="C404" s="20" t="s">
         <v>389</v>
       </c>
       <c r="D404" s="5"/>
@@ -6908,7 +6908,7 @@
       <c r="B405" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C405" s="19" t="s">
+      <c r="C405" s="20" t="s">
         <v>88</v>
       </c>
       <c r="D405" s="5"/>
@@ -6921,7 +6921,7 @@
       <c r="B406" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C406" s="19" t="s">
+      <c r="C406" s="20" t="s">
         <v>390</v>
       </c>
       <c r="D406" s="5"/>
@@ -6934,7 +6934,7 @@
       <c r="B407" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C407" s="19" t="s">
+      <c r="C407" s="20" t="s">
         <v>391</v>
       </c>
       <c r="D407" s="5"/>
@@ -6944,7 +6944,7 @@
         <f aca="false">A407 + 1</f>
         <v>403</v>
       </c>
-      <c r="C408" s="20"/>
+      <c r="C408" s="19"/>
       <c r="D408" s="5"/>
     </row>
     <row r="409" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6952,7 +6952,7 @@
         <f aca="false">A408 + 1</f>
         <v>404</v>
       </c>
-      <c r="C409" s="20"/>
+      <c r="C409" s="19"/>
       <c r="D409" s="5"/>
     </row>
     <row r="410" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6963,7 +6963,7 @@
       <c r="B410" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C410" s="19" t="s">
+      <c r="C410" s="20" t="s">
         <v>393</v>
       </c>
       <c r="D410" s="5"/>
@@ -6976,7 +6976,7 @@
       <c r="B411" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C411" s="19" t="s">
+      <c r="C411" s="20" t="s">
         <v>394</v>
       </c>
       <c r="D411" s="5"/>
@@ -6989,7 +6989,7 @@
       <c r="B412" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C412" s="19" t="s">
+      <c r="C412" s="20" t="s">
         <v>395</v>
       </c>
       <c r="D412" s="5"/>
@@ -7002,7 +7002,7 @@
       <c r="B413" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C413" s="19" t="s">
+      <c r="C413" s="20" t="s">
         <v>396</v>
       </c>
       <c r="D413" s="5"/>
@@ -7015,7 +7015,7 @@
       <c r="B414" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C414" s="19" t="s">
+      <c r="C414" s="20" t="s">
         <v>397</v>
       </c>
       <c r="D414" s="5"/>
@@ -7028,7 +7028,7 @@
       <c r="B415" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C415" s="19" t="s">
+      <c r="C415" s="20" t="s">
         <v>398</v>
       </c>
       <c r="D415" s="5"/>
@@ -7041,7 +7041,7 @@
       <c r="B416" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C416" s="19" t="s">
+      <c r="C416" s="20" t="s">
         <v>399</v>
       </c>
       <c r="D416" s="5"/>
@@ -7054,7 +7054,7 @@
       <c r="B417" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C417" s="19" t="s">
+      <c r="C417" s="20" t="s">
         <v>272</v>
       </c>
       <c r="D417" s="5"/>
@@ -7067,7 +7067,7 @@
       <c r="B418" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C418" s="19" t="s">
+      <c r="C418" s="20" t="s">
         <v>400</v>
       </c>
       <c r="D418" s="5"/>
@@ -7080,7 +7080,7 @@
       <c r="B419" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C419" s="19" t="s">
+      <c r="C419" s="20" t="s">
         <v>401</v>
       </c>
       <c r="D419" s="5"/>
@@ -7093,7 +7093,7 @@
       <c r="B420" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C420" s="19" t="s">
+      <c r="C420" s="20" t="s">
         <v>402</v>
       </c>
       <c r="D420" s="5"/>
@@ -7106,7 +7106,7 @@
       <c r="B421" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C421" s="19" t="s">
+      <c r="C421" s="20" t="s">
         <v>403</v>
       </c>
       <c r="D421" s="5"/>
@@ -7119,7 +7119,7 @@
       <c r="B422" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C422" s="19" t="s">
+      <c r="C422" s="20" t="s">
         <v>404</v>
       </c>
       <c r="D422" s="5"/>
@@ -7132,7 +7132,7 @@
       <c r="B423" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C423" s="19" t="s">
+      <c r="C423" s="20" t="s">
         <v>405</v>
       </c>
       <c r="D423" s="5"/>
@@ -7145,7 +7145,7 @@
       <c r="B424" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C424" s="19" t="s">
+      <c r="C424" s="20" t="s">
         <v>406</v>
       </c>
       <c r="D424" s="5"/>
@@ -7158,7 +7158,7 @@
       <c r="B425" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C425" s="19" t="s">
+      <c r="C425" s="20" t="s">
         <v>407</v>
       </c>
       <c r="D425" s="5"/>
@@ -7171,7 +7171,7 @@
       <c r="B426" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C426" s="19" t="s">
+      <c r="C426" s="20" t="s">
         <v>408</v>
       </c>
       <c r="D426" s="5"/>
@@ -7184,7 +7184,7 @@
       <c r="B427" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C427" s="19" t="s">
+      <c r="C427" s="20" t="s">
         <v>409</v>
       </c>
       <c r="D427" s="5"/>
@@ -7197,7 +7197,7 @@
       <c r="B428" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C428" s="19" t="s">
+      <c r="C428" s="20" t="s">
         <v>410</v>
       </c>
       <c r="D428" s="5"/>
@@ -7210,7 +7210,7 @@
       <c r="B429" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C429" s="19" t="s">
+      <c r="C429" s="20" t="s">
         <v>411</v>
       </c>
       <c r="D429" s="5"/>
@@ -7223,7 +7223,7 @@
       <c r="B430" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C430" s="19" t="s">
+      <c r="C430" s="20" t="s">
         <v>412</v>
       </c>
       <c r="D430" s="5"/>
@@ -7236,7 +7236,7 @@
       <c r="B431" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C431" s="19" t="s">
+      <c r="C431" s="20" t="s">
         <v>413</v>
       </c>
       <c r="D431" s="5"/>
@@ -7249,7 +7249,7 @@
       <c r="B432" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C432" s="19" t="s">
+      <c r="C432" s="20" t="s">
         <v>414</v>
       </c>
       <c r="D432" s="5"/>
@@ -7262,7 +7262,7 @@
       <c r="B433" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C433" s="19" t="s">
+      <c r="C433" s="20" t="s">
         <v>415</v>
       </c>
       <c r="D433" s="5"/>
@@ -7275,7 +7275,7 @@
       <c r="B434" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C434" s="19" t="s">
+      <c r="C434" s="20" t="s">
         <v>416</v>
       </c>
       <c r="D434" s="5"/>
@@ -7288,7 +7288,7 @@
       <c r="B435" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C435" s="19" t="s">
+      <c r="C435" s="20" t="s">
         <v>417</v>
       </c>
       <c r="D435" s="5"/>
@@ -7301,7 +7301,7 @@
       <c r="B436" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C436" s="19" t="s">
+      <c r="C436" s="20" t="s">
         <v>418</v>
       </c>
       <c r="D436" s="5"/>
@@ -7314,7 +7314,7 @@
       <c r="B437" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C437" s="19" t="s">
+      <c r="C437" s="20" t="s">
         <v>419</v>
       </c>
       <c r="D437" s="5"/>
@@ -7327,7 +7327,7 @@
       <c r="B438" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C438" s="19" t="s">
+      <c r="C438" s="20" t="s">
         <v>420</v>
       </c>
       <c r="D438" s="5"/>
@@ -7340,7 +7340,7 @@
       <c r="B439" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C439" s="19" t="s">
+      <c r="C439" s="20" t="s">
         <v>421</v>
       </c>
       <c r="D439" s="5"/>
@@ -7353,7 +7353,7 @@
       <c r="B440" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C440" s="19" t="s">
+      <c r="C440" s="20" t="s">
         <v>422</v>
       </c>
       <c r="D440" s="5"/>
@@ -7366,7 +7366,7 @@
       <c r="B441" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C441" s="19" t="s">
+      <c r="C441" s="20" t="s">
         <v>423</v>
       </c>
       <c r="D441" s="5"/>
@@ -7379,7 +7379,7 @@
       <c r="B442" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C442" s="19" t="s">
+      <c r="C442" s="20" t="s">
         <v>424</v>
       </c>
       <c r="D442" s="5"/>
@@ -7392,7 +7392,7 @@
       <c r="B443" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C443" s="19" t="s">
+      <c r="C443" s="20" t="s">
         <v>425</v>
       </c>
       <c r="D443" s="5"/>
@@ -7405,7 +7405,7 @@
       <c r="B444" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C444" s="19" t="s">
+      <c r="C444" s="20" t="s">
         <v>426</v>
       </c>
       <c r="D444" s="5"/>
@@ -7418,7 +7418,7 @@
       <c r="B445" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C445" s="19" t="s">
+      <c r="C445" s="20" t="s">
         <v>427</v>
       </c>
       <c r="D445" s="5"/>
@@ -7431,7 +7431,7 @@
       <c r="B446" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C446" s="19" t="s">
+      <c r="C446" s="20" t="s">
         <v>428</v>
       </c>
       <c r="D446" s="5"/>
@@ -7444,7 +7444,7 @@
       <c r="B447" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C447" s="19" t="s">
+      <c r="C447" s="20" t="s">
         <v>429</v>
       </c>
       <c r="D447" s="5"/>
@@ -7457,7 +7457,7 @@
       <c r="B448" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C448" s="19" t="s">
+      <c r="C448" s="20" t="s">
         <v>430</v>
       </c>
       <c r="D448" s="5"/>
@@ -7470,7 +7470,7 @@
       <c r="B449" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C449" s="19" t="s">
+      <c r="C449" s="20" t="s">
         <v>431</v>
       </c>
       <c r="D449" s="5"/>
@@ -7483,7 +7483,7 @@
       <c r="B450" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C450" s="19" t="s">
+      <c r="C450" s="20" t="s">
         <v>432</v>
       </c>
       <c r="D450" s="5"/>
@@ -7496,7 +7496,7 @@
       <c r="B451" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C451" s="19" t="s">
+      <c r="C451" s="20" t="s">
         <v>433</v>
       </c>
       <c r="D451" s="5"/>
@@ -7509,7 +7509,7 @@
       <c r="B452" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C452" s="19" t="s">
+      <c r="C452" s="20" t="s">
         <v>434</v>
       </c>
       <c r="D452" s="5"/>
@@ -7522,7 +7522,7 @@
       <c r="B453" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C453" s="19" t="s">
+      <c r="C453" s="20" t="s">
         <v>435</v>
       </c>
       <c r="D453" s="5"/>
@@ -7535,7 +7535,7 @@
       <c r="B454" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C454" s="19" t="s">
+      <c r="C454" s="20" t="s">
         <v>436</v>
       </c>
       <c r="D454" s="5"/>
@@ -7548,7 +7548,7 @@
       <c r="B455" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C455" s="19" t="s">
+      <c r="C455" s="20" t="s">
         <v>437</v>
       </c>
       <c r="D455" s="5"/>
@@ -7561,7 +7561,7 @@
       <c r="B456" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C456" s="19" t="s">
+      <c r="C456" s="20" t="s">
         <v>438</v>
       </c>
       <c r="D456" s="5"/>
@@ -7574,7 +7574,7 @@
       <c r="B457" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C457" s="19" t="s">
+      <c r="C457" s="20" t="s">
         <v>439</v>
       </c>
       <c r="D457" s="5"/>
@@ -7587,7 +7587,7 @@
       <c r="B458" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C458" s="19" t="s">
+      <c r="C458" s="20" t="s">
         <v>440</v>
       </c>
       <c r="D458" s="5"/>
@@ -7600,7 +7600,7 @@
       <c r="B459" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C459" s="19" t="s">
+      <c r="C459" s="20" t="s">
         <v>441</v>
       </c>
       <c r="D459" s="5"/>
@@ -7613,7 +7613,7 @@
       <c r="B460" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C460" s="19" t="s">
+      <c r="C460" s="20" t="s">
         <v>442</v>
       </c>
       <c r="D460" s="5"/>
@@ -7626,7 +7626,7 @@
       <c r="B461" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C461" s="19" t="s">
+      <c r="C461" s="20" t="s">
         <v>443</v>
       </c>
       <c r="D461" s="5"/>
@@ -7639,7 +7639,7 @@
       <c r="B462" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C462" s="19" t="s">
+      <c r="C462" s="20" t="s">
         <v>444</v>
       </c>
       <c r="D462" s="5"/>
@@ -7652,7 +7652,7 @@
       <c r="B463" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C463" s="19" t="s">
+      <c r="C463" s="20" t="s">
         <v>445</v>
       </c>
       <c r="D463" s="5"/>
@@ -7665,7 +7665,7 @@
       <c r="B464" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C464" s="19" t="s">
+      <c r="C464" s="20" t="s">
         <v>446</v>
       </c>
       <c r="D464" s="5"/>
@@ -7678,7 +7678,7 @@
       <c r="B465" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C465" s="19" t="s">
+      <c r="C465" s="20" t="s">
         <v>447</v>
       </c>
       <c r="D465" s="5"/>
@@ -7691,7 +7691,7 @@
       <c r="B466" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C466" s="19" t="s">
+      <c r="C466" s="20" t="s">
         <v>448</v>
       </c>
       <c r="D466" s="5"/>
@@ -7704,7 +7704,7 @@
       <c r="B467" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C467" s="19" t="s">
+      <c r="C467" s="20" t="s">
         <v>449</v>
       </c>
       <c r="D467" s="5"/>
@@ -7717,7 +7717,7 @@
       <c r="B468" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C468" s="19" t="s">
+      <c r="C468" s="20" t="s">
         <v>450</v>
       </c>
       <c r="D468" s="5"/>
@@ -7730,7 +7730,7 @@
       <c r="B469" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C469" s="19" t="s">
+      <c r="C469" s="20" t="s">
         <v>451</v>
       </c>
       <c r="D469" s="5"/>
@@ -7740,7 +7740,7 @@
         <f aca="false">A469 + 1</f>
         <v>465</v>
       </c>
-      <c r="C470" s="20"/>
+      <c r="C470" s="19"/>
       <c r="D470" s="5"/>
     </row>
     <row r="471" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7749,7 +7749,7 @@
         <v>466</v>
       </c>
       <c r="B471" s="15"/>
-      <c r="C471" s="20"/>
+      <c r="C471" s="19"/>
       <c r="D471" s="5"/>
     </row>
     <row r="472" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7760,7 +7760,7 @@
       <c r="B472" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C472" s="19" t="s">
+      <c r="C472" s="20" t="s">
         <v>453</v>
       </c>
       <c r="D472" s="5"/>
@@ -7773,7 +7773,7 @@
       <c r="B473" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C473" s="19" t="s">
+      <c r="C473" s="20" t="s">
         <v>454</v>
       </c>
       <c r="D473" s="5"/>
@@ -7786,7 +7786,7 @@
       <c r="B474" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C474" s="19" t="s">
+      <c r="C474" s="20" t="s">
         <v>455</v>
       </c>
       <c r="D474" s="5"/>
@@ -7799,7 +7799,7 @@
       <c r="B475" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C475" s="19" t="s">
+      <c r="C475" s="20" t="s">
         <v>456</v>
       </c>
       <c r="D475" s="5"/>
@@ -7812,7 +7812,7 @@
       <c r="B476" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C476" s="19" t="s">
+      <c r="C476" s="20" t="s">
         <v>457</v>
       </c>
       <c r="D476" s="5"/>
@@ -7825,7 +7825,7 @@
       <c r="B477" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C477" s="19" t="s">
+      <c r="C477" s="20" t="s">
         <v>458</v>
       </c>
       <c r="D477" s="5"/>
@@ -7838,7 +7838,7 @@
       <c r="B478" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C478" s="19" t="s">
+      <c r="C478" s="20" t="s">
         <v>459</v>
       </c>
       <c r="D478" s="5"/>
@@ -7851,7 +7851,7 @@
       <c r="B479" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C479" s="19" t="s">
+      <c r="C479" s="20" t="s">
         <v>460</v>
       </c>
       <c r="D479" s="5"/>
@@ -7864,7 +7864,7 @@
       <c r="B480" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C480" s="19" t="s">
+      <c r="C480" s="20" t="s">
         <v>461</v>
       </c>
       <c r="D480" s="5"/>
@@ -7877,7 +7877,7 @@
       <c r="B481" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="C481" s="19" t="s">
+      <c r="C481" s="20" t="s">
         <v>462</v>
       </c>
       <c r="D481" s="5"/>
@@ -7919,7 +7919,7 @@
     <hyperlink ref="C37" r:id="rId33" display="Three way partitioning of an array around a given value"/>
     <hyperlink ref="C38" r:id="rId34" display="Minimum swaps required bring elements less equal K together"/>
     <hyperlink ref="C39" r:id="rId35" display="Minimum no. of operations required to make an array palindrome"/>
-    <hyperlink ref="C40" r:id="rId36" display="Median of 2 sorted arrays of equal size"/>
+    <hyperlink ref="C40" r:id="rId36" location=":~:text=Method%201%20(Simply%20count%20while,n%20in%20the%20merged%20array." display="Median of 2 sorted arrays of equal size"/>
     <hyperlink ref="C41" r:id="rId37" display="Median of 2 sorted arrays of different size"/>
     <hyperlink ref="C44" r:id="rId38" display="Spiral traversal on a Matrix"/>
     <hyperlink ref="C45" r:id="rId39" display="Search an element in a matriix"/>

</xml_diff>